<commit_message>
Change wrong unit/number in cumBg call in IlSBMP2
</commit_message>
<xml_diff>
--- a/experiments/IISBMP2/data/biogas_and_setup.xlsx
+++ b/experiments/IISBMP2/data/biogas_and_setup.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16395" windowHeight="8190" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16395" windowHeight="8190" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="1" r:id="rId1"/>
@@ -2492,11 +2492,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK240"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B60" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H3" sqref="H3:H16"/>
+      <selection pane="bottomRight" activeCell="G74" sqref="G74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2630,7 +2630,7 @@
         <v>43370.649305555555</v>
       </c>
       <c r="L3" s="6">
-        <f>K3-K$3</f>
+        <f t="shared" ref="L3:L66" si="0">K3-K$3</f>
         <v>0</v>
       </c>
     </row>
@@ -2670,7 +2670,7 @@
         <v>43370.649305555598</v>
       </c>
       <c r="L4" s="6">
-        <f>K4-K$3</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2710,7 +2710,7 @@
         <v>43370.649305555598</v>
       </c>
       <c r="L5" s="6">
-        <f>K5-K$3</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2750,7 +2750,7 @@
         <v>43370.649305555598</v>
       </c>
       <c r="L6" s="6">
-        <f>K6-K$3</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2790,7 +2790,7 @@
         <v>43370.649305555598</v>
       </c>
       <c r="L7" s="6">
-        <f>K7-K$3</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2830,7 +2830,7 @@
         <v>43370.649305555598</v>
       </c>
       <c r="L8" s="6">
-        <f>K8-K$3</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2870,7 +2870,7 @@
         <v>43370.649305555598</v>
       </c>
       <c r="L9" s="6">
-        <f>K9-K$3</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2910,7 +2910,7 @@
         <v>43370.649305555598</v>
       </c>
       <c r="L10" s="6">
-        <f>K10-K$3</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2950,7 +2950,7 @@
         <v>43370.649305555598</v>
       </c>
       <c r="L11" s="6">
-        <f>K11-K$3</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2990,7 +2990,7 @@
         <v>43370.649305555598</v>
       </c>
       <c r="L12" s="6">
-        <f>K12-K$3</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3030,7 +3030,7 @@
         <v>43370.649305555598</v>
       </c>
       <c r="L13" s="6">
-        <f>K13-K$3</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3070,7 +3070,7 @@
         <v>43370.649305555598</v>
       </c>
       <c r="L14" s="6">
-        <f>K14-K$3</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3110,7 +3110,7 @@
         <v>43370.649305555598</v>
       </c>
       <c r="L15" s="6">
-        <f>K15-K$3</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3150,7 +3150,7 @@
         <v>43370.649305555598</v>
       </c>
       <c r="L16" s="6">
-        <f>K16-K$3</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3187,7 +3187,7 @@
         <v>43371.375</v>
       </c>
       <c r="L17" s="6">
-        <f>K17-K$3</f>
+        <f t="shared" si="0"/>
         <v>0.72569444444525288</v>
       </c>
     </row>
@@ -3224,7 +3224,7 @@
         <v>43371.375</v>
       </c>
       <c r="L18" s="6">
-        <f>K18-K$3</f>
+        <f t="shared" si="0"/>
         <v>0.72569444444525288</v>
       </c>
     </row>
@@ -3261,7 +3261,7 @@
         <v>43371.375</v>
       </c>
       <c r="L19" s="6">
-        <f>K19-K$3</f>
+        <f t="shared" si="0"/>
         <v>0.72569444444525288</v>
       </c>
     </row>
@@ -3294,7 +3294,7 @@
         <v>43371.375</v>
       </c>
       <c r="L20" s="6">
-        <f>K20-K$3</f>
+        <f t="shared" si="0"/>
         <v>0.72569444444525288</v>
       </c>
     </row>
@@ -3334,7 +3334,7 @@
         <v>43371.375</v>
       </c>
       <c r="L21" s="6">
-        <f>K21-K$3</f>
+        <f t="shared" si="0"/>
         <v>0.72569444444525288</v>
       </c>
     </row>
@@ -3371,7 +3371,7 @@
         <v>43371.375</v>
       </c>
       <c r="L22" s="6">
-        <f>K22-K$3</f>
+        <f t="shared" si="0"/>
         <v>0.72569444444525288</v>
       </c>
     </row>
@@ -3408,7 +3408,7 @@
         <v>43371.375</v>
       </c>
       <c r="L23" s="6">
-        <f>K23-K$3</f>
+        <f t="shared" si="0"/>
         <v>0.72569444444525288</v>
       </c>
     </row>
@@ -3445,7 +3445,7 @@
         <v>43371.375</v>
       </c>
       <c r="L24" s="6">
-        <f>K24-K$3</f>
+        <f t="shared" si="0"/>
         <v>0.72569444444525288</v>
       </c>
     </row>
@@ -3481,7 +3481,7 @@
         <v>43371.375</v>
       </c>
       <c r="L25" s="6">
-        <f>K25-K$3</f>
+        <f t="shared" si="0"/>
         <v>0.72569444444525288</v>
       </c>
     </row>
@@ -3517,7 +3517,7 @@
         <v>43371.375</v>
       </c>
       <c r="L26" s="6">
-        <f>K26-K$3</f>
+        <f t="shared" si="0"/>
         <v>0.72569444444525288</v>
       </c>
     </row>
@@ -3556,7 +3556,7 @@
         <v>43371.375</v>
       </c>
       <c r="L27" s="6">
-        <f>K27-K$3</f>
+        <f t="shared" si="0"/>
         <v>0.72569444444525288</v>
       </c>
     </row>
@@ -3595,7 +3595,7 @@
         <v>43371.375</v>
       </c>
       <c r="L28" s="6">
-        <f>K28-K$3</f>
+        <f t="shared" si="0"/>
         <v>0.72569444444525288</v>
       </c>
     </row>
@@ -3634,7 +3634,7 @@
         <v>43371.375</v>
       </c>
       <c r="L29" s="6">
-        <f>K29-K$3</f>
+        <f t="shared" si="0"/>
         <v>0.72569444444525288</v>
       </c>
     </row>
@@ -3673,7 +3673,7 @@
         <v>43371.375</v>
       </c>
       <c r="L30" s="6">
-        <f>K30-K$3</f>
+        <f t="shared" si="0"/>
         <v>0.72569444444525288</v>
       </c>
     </row>
@@ -3710,7 +3710,7 @@
         <v>43372.253472222197</v>
       </c>
       <c r="L31" s="6">
-        <f>K31-K$3</f>
+        <f t="shared" si="0"/>
         <v>1.6041666666424135</v>
       </c>
     </row>
@@ -3749,7 +3749,7 @@
         <v>43372.253472222197</v>
       </c>
       <c r="L32" s="6">
-        <f>K32-K$3</f>
+        <f t="shared" si="0"/>
         <v>1.6041666666424135</v>
       </c>
     </row>
@@ -3788,7 +3788,7 @@
         <v>43372.253472222197</v>
       </c>
       <c r="L33" s="6">
-        <f>K33-K$3</f>
+        <f t="shared" si="0"/>
         <v>1.6041666666424135</v>
       </c>
     </row>
@@ -3827,7 +3827,7 @@
         <v>43372.253472222197</v>
       </c>
       <c r="L34" s="6">
-        <f>K34-K$3</f>
+        <f t="shared" si="0"/>
         <v>1.6041666666424135</v>
       </c>
     </row>
@@ -3866,7 +3866,7 @@
         <v>43372.253472222197</v>
       </c>
       <c r="L35" s="6">
-        <f>K35-K$3</f>
+        <f t="shared" si="0"/>
         <v>1.6041666666424135</v>
       </c>
     </row>
@@ -3905,7 +3905,7 @@
         <v>43372.253472222197</v>
       </c>
       <c r="L36" s="6">
-        <f>K36-K$3</f>
+        <f t="shared" si="0"/>
         <v>1.6041666666424135</v>
       </c>
     </row>
@@ -3944,7 +3944,7 @@
         <v>43372.253472222197</v>
       </c>
       <c r="L37" s="6">
-        <f>K37-K$3</f>
+        <f t="shared" si="0"/>
         <v>1.6041666666424135</v>
       </c>
     </row>
@@ -3983,7 +3983,7 @@
         <v>43372.253472222197</v>
       </c>
       <c r="L38" s="6">
-        <f>K38-K$3</f>
+        <f t="shared" si="0"/>
         <v>1.6041666666424135</v>
       </c>
     </row>
@@ -4023,7 +4023,7 @@
         <v>43372.253472222197</v>
       </c>
       <c r="L39" s="6">
-        <f>K39-K$3</f>
+        <f t="shared" si="0"/>
         <v>1.6041666666424135</v>
       </c>
     </row>
@@ -4063,7 +4063,7 @@
         <v>43372.253472222197</v>
       </c>
       <c r="L40" s="6">
-        <f>K40-K$3</f>
+        <f t="shared" si="0"/>
         <v>1.6041666666424135</v>
       </c>
     </row>
@@ -4103,7 +4103,7 @@
         <v>43372.253472222197</v>
       </c>
       <c r="L41" s="6">
-        <f>K41-K$3</f>
+        <f t="shared" si="0"/>
         <v>1.6041666666424135</v>
       </c>
     </row>
@@ -4143,7 +4143,7 @@
         <v>43372.253472222197</v>
       </c>
       <c r="L42" s="6">
-        <f>K42-K$3</f>
+        <f t="shared" si="0"/>
         <v>1.6041666666424135</v>
       </c>
     </row>
@@ -4183,7 +4183,7 @@
         <v>43372.253472222197</v>
       </c>
       <c r="L43" s="6">
-        <f>K43-K$3</f>
+        <f t="shared" si="0"/>
         <v>1.6041666666424135</v>
       </c>
     </row>
@@ -4223,7 +4223,7 @@
         <v>43372.253472222197</v>
       </c>
       <c r="L44" s="6">
-        <f>K44-K$3</f>
+        <f t="shared" si="0"/>
         <v>1.6041666666424135</v>
       </c>
     </row>
@@ -4260,7 +4260,7 @@
         <v>43373.626388888901</v>
       </c>
       <c r="L45" s="6">
-        <f>K45-K$3</f>
+        <f t="shared" si="0"/>
         <v>2.977083333345945</v>
       </c>
     </row>
@@ -4297,7 +4297,7 @@
         <v>43373.626388888901</v>
       </c>
       <c r="L46" s="6">
-        <f>K46-K$3</f>
+        <f t="shared" si="0"/>
         <v>2.977083333345945</v>
       </c>
     </row>
@@ -4334,7 +4334,7 @@
         <v>43373.626388888901</v>
       </c>
       <c r="L47" s="6">
-        <f>K47-K$3</f>
+        <f t="shared" si="0"/>
         <v>2.977083333345945</v>
       </c>
     </row>
@@ -4370,7 +4370,7 @@
         <v>43373.626388888901</v>
       </c>
       <c r="L48" s="6">
-        <f>K48-K$3</f>
+        <f t="shared" si="0"/>
         <v>2.977083333345945</v>
       </c>
     </row>
@@ -4407,7 +4407,7 @@
         <v>43373.626388888901</v>
       </c>
       <c r="L49" s="6">
-        <f>K49-K$3</f>
+        <f t="shared" si="0"/>
         <v>2.977083333345945</v>
       </c>
     </row>
@@ -4444,7 +4444,7 @@
         <v>43373.626388888901</v>
       </c>
       <c r="L50" s="6">
-        <f>K50-K$3</f>
+        <f t="shared" si="0"/>
         <v>2.977083333345945</v>
       </c>
     </row>
@@ -4481,7 +4481,7 @@
         <v>43373.626388888901</v>
       </c>
       <c r="L51" s="6">
-        <f>K51-K$3</f>
+        <f t="shared" si="0"/>
         <v>2.977083333345945</v>
       </c>
     </row>
@@ -4518,7 +4518,7 @@
         <v>43373.626388888901</v>
       </c>
       <c r="L52" s="6">
-        <f>K52-K$3</f>
+        <f t="shared" si="0"/>
         <v>2.977083333345945</v>
       </c>
     </row>
@@ -4555,7 +4555,7 @@
         <v>43373.626388888901</v>
       </c>
       <c r="L53" s="6">
-        <f>K53-K$3</f>
+        <f t="shared" si="0"/>
         <v>2.977083333345945</v>
       </c>
     </row>
@@ -4592,7 +4592,7 @@
         <v>43373.626388888901</v>
       </c>
       <c r="L54" s="6">
-        <f>K54-K$3</f>
+        <f t="shared" si="0"/>
         <v>2.977083333345945</v>
       </c>
     </row>
@@ -4632,7 +4632,7 @@
         <v>43373.626388888901</v>
       </c>
       <c r="L55" s="6">
-        <f>K55-K$3</f>
+        <f t="shared" si="0"/>
         <v>2.977083333345945</v>
       </c>
     </row>
@@ -4672,7 +4672,7 @@
         <v>43373.626388888901</v>
       </c>
       <c r="L56" s="6">
-        <f>K56-K$3</f>
+        <f t="shared" si="0"/>
         <v>2.977083333345945</v>
       </c>
     </row>
@@ -4711,7 +4711,7 @@
         <v>43373.626388888901</v>
       </c>
       <c r="L57" s="6">
-        <f>K57-K$3</f>
+        <f t="shared" si="0"/>
         <v>2.977083333345945</v>
       </c>
     </row>
@@ -4750,7 +4750,7 @@
         <v>43373.626388888901</v>
       </c>
       <c r="L58" s="6">
-        <f>K58-K$3</f>
+        <f t="shared" si="0"/>
         <v>2.977083333345945</v>
       </c>
     </row>
@@ -4786,7 +4786,7 @@
         <v>43374.368055555598</v>
       </c>
       <c r="L59" s="6">
-        <f>K59-K$3</f>
+        <f t="shared" si="0"/>
         <v>3.7187500000436557</v>
       </c>
     </row>
@@ -4825,7 +4825,7 @@
         <v>43374.368055555598</v>
       </c>
       <c r="L60" s="6">
-        <f>K60-K$3</f>
+        <f t="shared" si="0"/>
         <v>3.7187500000436557</v>
       </c>
     </row>
@@ -4861,7 +4861,7 @@
         <v>43374.368055555598</v>
       </c>
       <c r="L61" s="6">
-        <f>K61-K$3</f>
+        <f t="shared" si="0"/>
         <v>3.7187500000436557</v>
       </c>
     </row>
@@ -4897,7 +4897,7 @@
         <v>43374.368055555598</v>
       </c>
       <c r="L62" s="6">
-        <f>K62-K$3</f>
+        <f t="shared" si="0"/>
         <v>3.7187500000436557</v>
       </c>
     </row>
@@ -4933,7 +4933,7 @@
         <v>43374.368055555598</v>
       </c>
       <c r="L63" s="6">
-        <f>K63-K$3</f>
+        <f t="shared" si="0"/>
         <v>3.7187500000436557</v>
       </c>
     </row>
@@ -4970,7 +4970,7 @@
         <v>43374.368055555598</v>
       </c>
       <c r="L64" s="6">
-        <f>K64-K$3</f>
+        <f t="shared" si="0"/>
         <v>3.7187500000436557</v>
       </c>
     </row>
@@ -5007,7 +5007,7 @@
         <v>43374.368055555598</v>
       </c>
       <c r="L65" s="6">
-        <f>K65-K$3</f>
+        <f t="shared" si="0"/>
         <v>3.7187500000436557</v>
       </c>
     </row>
@@ -5044,7 +5044,7 @@
         <v>43374.368055555598</v>
       </c>
       <c r="L66" s="6">
-        <f>K66-K$3</f>
+        <f t="shared" si="0"/>
         <v>3.7187500000436557</v>
       </c>
     </row>
@@ -5081,7 +5081,7 @@
         <v>43374.368055555598</v>
       </c>
       <c r="L67" s="6">
-        <f>K67-K$3</f>
+        <f t="shared" ref="L67:L130" si="1">K67-K$3</f>
         <v>3.7187500000436557</v>
       </c>
     </row>
@@ -5118,7 +5118,7 @@
         <v>43374.368055555598</v>
       </c>
       <c r="L68" s="6">
-        <f>K68-K$3</f>
+        <f t="shared" si="1"/>
         <v>3.7187500000436557</v>
       </c>
     </row>
@@ -5155,7 +5155,7 @@
         <v>43374.368055555598</v>
       </c>
       <c r="L69" s="6">
-        <f>K69-K$3</f>
+        <f t="shared" si="1"/>
         <v>3.7187500000436557</v>
       </c>
     </row>
@@ -5192,7 +5192,7 @@
         <v>43374.368055555598</v>
       </c>
       <c r="L70" s="6">
-        <f>K70-K$3</f>
+        <f t="shared" si="1"/>
         <v>3.7187500000436557</v>
       </c>
     </row>
@@ -5229,7 +5229,7 @@
         <v>43374.368055555598</v>
       </c>
       <c r="L71" s="6">
-        <f>K71-K$3</f>
+        <f t="shared" si="1"/>
         <v>3.7187500000436557</v>
       </c>
     </row>
@@ -5266,7 +5266,7 @@
         <v>43374.368055555598</v>
       </c>
       <c r="L72" s="6">
-        <f>K72-K$3</f>
+        <f t="shared" si="1"/>
         <v>3.7187500000436557</v>
       </c>
     </row>
@@ -5299,7 +5299,7 @@
         <v>43375.40625</v>
       </c>
       <c r="L73" s="6">
-        <f>K73-K$3</f>
+        <f t="shared" si="1"/>
         <v>4.7569444444452529</v>
       </c>
     </row>
@@ -5337,7 +5337,7 @@
         <v>43375.40625</v>
       </c>
       <c r="L74" s="6">
-        <f>K74-K$3</f>
+        <f t="shared" si="1"/>
         <v>4.7569444444452529</v>
       </c>
     </row>
@@ -5377,7 +5377,7 @@
         <v>43375.40625</v>
       </c>
       <c r="L75" s="6">
-        <f>K75-K$3</f>
+        <f t="shared" si="1"/>
         <v>4.7569444444452529</v>
       </c>
     </row>
@@ -5417,7 +5417,7 @@
         <v>43375.40625</v>
       </c>
       <c r="L76" s="6">
-        <f>K76-K$3</f>
+        <f t="shared" si="1"/>
         <v>4.7569444444452529</v>
       </c>
     </row>
@@ -5450,7 +5450,7 @@
         <v>43376.338194444397</v>
       </c>
       <c r="L77" s="6">
-        <f>K77-K$3</f>
+        <f t="shared" si="1"/>
         <v>5.6888888888424844</v>
       </c>
     </row>
@@ -5487,7 +5487,7 @@
         <v>43376.338194444397</v>
       </c>
       <c r="L78" s="6">
-        <f>K78-K$3</f>
+        <f t="shared" si="1"/>
         <v>5.6888888888424844</v>
       </c>
     </row>
@@ -5523,7 +5523,7 @@
         <v>43376.338194444397</v>
       </c>
       <c r="L79" s="6">
-        <f>K79-K$3</f>
+        <f t="shared" si="1"/>
         <v>5.6888888888424844</v>
       </c>
     </row>
@@ -5559,7 +5559,7 @@
         <v>43376.338194444397</v>
       </c>
       <c r="L80" s="6">
-        <f>K80-K$3</f>
+        <f t="shared" si="1"/>
         <v>5.6888888888424844</v>
       </c>
     </row>
@@ -5596,7 +5596,7 @@
         <v>43376.338194444397</v>
       </c>
       <c r="L81" s="6">
-        <f>K81-K$3</f>
+        <f t="shared" si="1"/>
         <v>5.6888888888424844</v>
       </c>
     </row>
@@ -5635,7 +5635,7 @@
         <v>43376.338194444397</v>
       </c>
       <c r="L82" s="6">
-        <f>K82-K$3</f>
+        <f t="shared" si="1"/>
         <v>5.6888888888424844</v>
       </c>
     </row>
@@ -5674,7 +5674,7 @@
         <v>43376.338194444397</v>
       </c>
       <c r="L83" s="6">
-        <f>K83-K$3</f>
+        <f t="shared" si="1"/>
         <v>5.6888888888424844</v>
       </c>
     </row>
@@ -5711,7 +5711,7 @@
         <v>43376.338194444397</v>
       </c>
       <c r="L84" s="6">
-        <f>K84-K$3</f>
+        <f t="shared" si="1"/>
         <v>5.6888888888424844</v>
       </c>
     </row>
@@ -5748,7 +5748,7 @@
         <v>43376.338194444397</v>
       </c>
       <c r="L85" s="6">
-        <f>K85-K$3</f>
+        <f t="shared" si="1"/>
         <v>5.6888888888424844</v>
       </c>
     </row>
@@ -5785,7 +5785,7 @@
         <v>43376.338194444397</v>
       </c>
       <c r="L86" s="6">
-        <f>K86-K$3</f>
+        <f t="shared" si="1"/>
         <v>5.6888888888424844</v>
       </c>
     </row>
@@ -5822,7 +5822,7 @@
         <v>43376.338194444397</v>
       </c>
       <c r="L87" s="6">
-        <f>K87-K$3</f>
+        <f t="shared" si="1"/>
         <v>5.6888888888424844</v>
       </c>
     </row>
@@ -5859,7 +5859,7 @@
         <v>43376.338194444397</v>
       </c>
       <c r="L88" s="6">
-        <f>K88-K$3</f>
+        <f t="shared" si="1"/>
         <v>5.6888888888424844</v>
       </c>
     </row>
@@ -5896,7 +5896,7 @@
         <v>43376.338194444397</v>
       </c>
       <c r="L89" s="6">
-        <f>K89-K$3</f>
+        <f t="shared" si="1"/>
         <v>5.6888888888424844</v>
       </c>
     </row>
@@ -5933,7 +5933,7 @@
         <v>43376.338194444397</v>
       </c>
       <c r="L90" s="6">
-        <f>K90-K$3</f>
+        <f t="shared" si="1"/>
         <v>5.6888888888424844</v>
       </c>
     </row>
@@ -5966,7 +5966,7 @@
         <v>43378.464583333298</v>
       </c>
       <c r="L91" s="6">
-        <f>K91-K$3</f>
+        <f t="shared" si="1"/>
         <v>7.8152777777431766</v>
       </c>
     </row>
@@ -6002,7 +6002,7 @@
         <v>43378.464583333298</v>
       </c>
       <c r="L92" s="6">
-        <f>K92-K$3</f>
+        <f t="shared" si="1"/>
         <v>7.8152777777431766</v>
       </c>
     </row>
@@ -6038,7 +6038,7 @@
         <v>43378.464583333298</v>
       </c>
       <c r="L93" s="6">
-        <f>K93-K$3</f>
+        <f t="shared" si="1"/>
         <v>7.8152777777431766</v>
       </c>
     </row>
@@ -6074,7 +6074,7 @@
         <v>43378.464583333298</v>
       </c>
       <c r="L94" s="6">
-        <f>K94-K$3</f>
+        <f t="shared" si="1"/>
         <v>7.8152777777431766</v>
       </c>
     </row>
@@ -6110,7 +6110,7 @@
         <v>43378.464583333298</v>
       </c>
       <c r="L95" s="6">
-        <f>K95-K$3</f>
+        <f t="shared" si="1"/>
         <v>7.8152777777431766</v>
       </c>
     </row>
@@ -6146,7 +6146,7 @@
         <v>43378.464583333298</v>
       </c>
       <c r="L96" s="6">
-        <f>K96-K$3</f>
+        <f t="shared" si="1"/>
         <v>7.8152777777431766</v>
       </c>
     </row>
@@ -6182,7 +6182,7 @@
         <v>43378.464583333298</v>
       </c>
       <c r="L97" s="6">
-        <f>K97-K$3</f>
+        <f t="shared" si="1"/>
         <v>7.8152777777431766</v>
       </c>
     </row>
@@ -6218,7 +6218,7 @@
         <v>43378.464583333298</v>
       </c>
       <c r="L98" s="6">
-        <f>K98-K$3</f>
+        <f t="shared" si="1"/>
         <v>7.8152777777431766</v>
       </c>
     </row>
@@ -6255,7 +6255,7 @@
         <v>43378.464583333298</v>
       </c>
       <c r="L99" s="6">
-        <f>K99-K$3</f>
+        <f t="shared" si="1"/>
         <v>7.8152777777431766</v>
       </c>
     </row>
@@ -6295,7 +6295,7 @@
         <v>43378.464583333298</v>
       </c>
       <c r="L100" s="6">
-        <f>K100-K$3</f>
+        <f t="shared" si="1"/>
         <v>7.8152777777431766</v>
       </c>
     </row>
@@ -6332,7 +6332,7 @@
         <v>43378.464583333298</v>
       </c>
       <c r="L101" s="6">
-        <f>K101-K$3</f>
+        <f t="shared" si="1"/>
         <v>7.8152777777431766</v>
       </c>
     </row>
@@ -6368,7 +6368,7 @@
         <v>43378.464583333298</v>
       </c>
       <c r="L102" s="6">
-        <f>K102-K$3</f>
+        <f t="shared" si="1"/>
         <v>7.8152777777431766</v>
       </c>
     </row>
@@ -6404,7 +6404,7 @@
         <v>43378.464583333298</v>
       </c>
       <c r="L103" s="6">
-        <f>K103-K$3</f>
+        <f t="shared" si="1"/>
         <v>7.8152777777431766</v>
       </c>
     </row>
@@ -6440,7 +6440,7 @@
         <v>43378.464583333298</v>
       </c>
       <c r="L104" s="6">
-        <f>K104-K$3</f>
+        <f t="shared" si="1"/>
         <v>7.8152777777431766</v>
       </c>
     </row>
@@ -6476,7 +6476,7 @@
         <v>43379.888888888898</v>
       </c>
       <c r="L105" s="6">
-        <f>K105-K$3</f>
+        <f t="shared" si="1"/>
         <v>9.2395833333430346</v>
       </c>
     </row>
@@ -6513,7 +6513,7 @@
         <v>43379.888888888898</v>
       </c>
       <c r="L106" s="6">
-        <f>K106-K$3</f>
+        <f t="shared" si="1"/>
         <v>9.2395833333430346</v>
       </c>
     </row>
@@ -6550,7 +6550,7 @@
         <v>43379.888888888898</v>
       </c>
       <c r="L107" s="6">
-        <f>K107-K$3</f>
+        <f t="shared" si="1"/>
         <v>9.2395833333430346</v>
       </c>
     </row>
@@ -6587,7 +6587,7 @@
         <v>43379.888888888898</v>
       </c>
       <c r="L108" s="6">
-        <f>K108-K$3</f>
+        <f t="shared" si="1"/>
         <v>9.2395833333430346</v>
       </c>
     </row>
@@ -6623,7 +6623,7 @@
         <v>43379.888888888898</v>
       </c>
       <c r="L109" s="6">
-        <f>K109-K$3</f>
+        <f t="shared" si="1"/>
         <v>9.2395833333430346</v>
       </c>
     </row>
@@ -6659,7 +6659,7 @@
         <v>43379.888888888898</v>
       </c>
       <c r="L110" s="6">
-        <f>K110-K$3</f>
+        <f t="shared" si="1"/>
         <v>9.2395833333430346</v>
       </c>
     </row>
@@ -6695,7 +6695,7 @@
         <v>43379.888888888898</v>
       </c>
       <c r="L111" s="6">
-        <f>K111-K$3</f>
+        <f t="shared" si="1"/>
         <v>9.2395833333430346</v>
       </c>
     </row>
@@ -6731,7 +6731,7 @@
         <v>43379.888888888898</v>
       </c>
       <c r="L112" s="6">
-        <f>K112-K$3</f>
+        <f t="shared" si="1"/>
         <v>9.2395833333430346</v>
       </c>
     </row>
@@ -6764,7 +6764,7 @@
         <v>43381.488194444399</v>
       </c>
       <c r="L113" s="6">
-        <f>K113-K$3</f>
+        <f t="shared" si="1"/>
         <v>10.83888888884394</v>
       </c>
     </row>
@@ -6800,7 +6800,7 @@
         <v>43381.488194444399</v>
       </c>
       <c r="L114" s="6">
-        <f>K114-K$3</f>
+        <f t="shared" si="1"/>
         <v>10.83888888884394</v>
       </c>
     </row>
@@ -6836,7 +6836,7 @@
         <v>43381.488194444399</v>
       </c>
       <c r="L115" s="6">
-        <f>K115-K$3</f>
+        <f t="shared" si="1"/>
         <v>10.83888888884394</v>
       </c>
     </row>
@@ -6872,7 +6872,7 @@
         <v>43381.488194444399</v>
       </c>
       <c r="L116" s="6">
-        <f>K116-K$3</f>
+        <f t="shared" si="1"/>
         <v>10.83888888884394</v>
       </c>
     </row>
@@ -6908,7 +6908,7 @@
         <v>43381.488194444399</v>
       </c>
       <c r="L117" s="6">
-        <f>K117-K$3</f>
+        <f t="shared" si="1"/>
         <v>10.83888888884394</v>
       </c>
     </row>
@@ -6944,7 +6944,7 @@
         <v>43381.488194444399</v>
       </c>
       <c r="L118" s="6">
-        <f>K118-K$3</f>
+        <f t="shared" si="1"/>
         <v>10.83888888884394</v>
       </c>
     </row>
@@ -6980,7 +6980,7 @@
         <v>43381.488194444399</v>
       </c>
       <c r="L119" s="6">
-        <f>K119-K$3</f>
+        <f t="shared" si="1"/>
         <v>10.83888888884394</v>
       </c>
     </row>
@@ -7016,7 +7016,7 @@
         <v>43381.488194444399</v>
       </c>
       <c r="L120" s="6">
-        <f>K120-K$3</f>
+        <f t="shared" si="1"/>
         <v>10.83888888884394</v>
       </c>
     </row>
@@ -7053,7 +7053,7 @@
         <v>43381.488194444399</v>
       </c>
       <c r="L121" s="6">
-        <f>K121-K$3</f>
+        <f t="shared" si="1"/>
         <v>10.83888888884394</v>
       </c>
     </row>
@@ -7090,7 +7090,7 @@
         <v>43381.488194444399</v>
       </c>
       <c r="L122" s="6">
-        <f>K122-K$3</f>
+        <f t="shared" si="1"/>
         <v>10.83888888884394</v>
       </c>
     </row>
@@ -7127,7 +7127,7 @@
         <v>43381.488194444399</v>
       </c>
       <c r="L123" s="6">
-        <f>K123-K$3</f>
+        <f t="shared" si="1"/>
         <v>10.83888888884394</v>
       </c>
     </row>
@@ -7163,7 +7163,7 @@
         <v>43381.488194444399</v>
       </c>
       <c r="L124" s="6">
-        <f>K124-K$3</f>
+        <f t="shared" si="1"/>
         <v>10.83888888884394</v>
       </c>
     </row>
@@ -7199,7 +7199,7 @@
         <v>43381.488194444399</v>
       </c>
       <c r="L125" s="6">
-        <f>K125-K$3</f>
+        <f t="shared" si="1"/>
         <v>10.83888888884394</v>
       </c>
     </row>
@@ -7235,7 +7235,7 @@
         <v>43381.488194444399</v>
       </c>
       <c r="L126" s="6">
-        <f>K126-K$3</f>
+        <f t="shared" si="1"/>
         <v>10.83888888884394</v>
       </c>
     </row>
@@ -7268,7 +7268,7 @@
         <v>43384.5090277778</v>
       </c>
       <c r="L127" s="6">
-        <f>K127-K$3</f>
+        <f t="shared" si="1"/>
         <v>13.859722222245182</v>
       </c>
     </row>
@@ -7304,7 +7304,7 @@
         <v>43384.509722222203</v>
       </c>
       <c r="L128" s="6">
-        <f>K128-K$3</f>
+        <f t="shared" si="1"/>
         <v>13.860416666648234</v>
       </c>
     </row>
@@ -7340,7 +7340,7 @@
         <v>43384.510416666701</v>
       </c>
       <c r="L129" s="6">
-        <f>K129-K$3</f>
+        <f t="shared" si="1"/>
         <v>13.861111111145874</v>
       </c>
     </row>
@@ -7376,7 +7376,7 @@
         <v>43384.511111111096</v>
       </c>
       <c r="L130" s="6">
-        <f>K130-K$3</f>
+        <f t="shared" si="1"/>
         <v>13.86180555554165</v>
       </c>
     </row>
@@ -7413,7 +7413,7 @@
         <v>43384.511805555601</v>
       </c>
       <c r="L131" s="6">
-        <f>K131-K$3</f>
+        <f t="shared" ref="L131:L194" si="2">K131-K$3</f>
         <v>13.862500000046566</v>
       </c>
     </row>
@@ -7450,7 +7450,7 @@
         <v>43384.512499999997</v>
       </c>
       <c r="L132" s="6">
-        <f>K132-K$3</f>
+        <f t="shared" si="2"/>
         <v>13.863194444442343</v>
       </c>
     </row>
@@ -7487,7 +7487,7 @@
         <v>43384.5131944444</v>
       </c>
       <c r="L133" s="6">
-        <f>K133-K$3</f>
+        <f t="shared" si="2"/>
         <v>13.863888888845395</v>
       </c>
     </row>
@@ -7524,7 +7524,7 @@
         <v>43384.513888888898</v>
       </c>
       <c r="L134" s="6">
-        <f>K134-K$3</f>
+        <f t="shared" si="2"/>
         <v>13.864583333343035</v>
       </c>
     </row>
@@ -7561,7 +7561,7 @@
         <v>43384.514583333301</v>
       </c>
       <c r="L135" s="6">
-        <f>K135-K$3</f>
+        <f t="shared" si="2"/>
         <v>13.865277777746087</v>
       </c>
     </row>
@@ -7598,7 +7598,7 @@
         <v>43384.515277777798</v>
       </c>
       <c r="L136" s="6">
-        <f>K136-K$3</f>
+        <f t="shared" si="2"/>
         <v>13.865972222243727</v>
       </c>
     </row>
@@ -7635,7 +7635,7 @@
         <v>43384.515972222202</v>
       </c>
       <c r="L137" s="6">
-        <f>K137-K$3</f>
+        <f t="shared" si="2"/>
         <v>13.866666666646779</v>
       </c>
     </row>
@@ -7671,7 +7671,7 @@
         <v>43384.516666666699</v>
       </c>
       <c r="L138" s="6">
-        <f>K138-K$3</f>
+        <f t="shared" si="2"/>
         <v>13.867361111144419</v>
       </c>
     </row>
@@ -7707,7 +7707,7 @@
         <v>43384.517361111102</v>
       </c>
       <c r="L139" s="6">
-        <f>K139-K$3</f>
+        <f t="shared" si="2"/>
         <v>13.868055555547471</v>
       </c>
     </row>
@@ -7743,7 +7743,7 @@
         <v>43384.5180555556</v>
       </c>
       <c r="L140" s="6">
-        <f>K140-K$3</f>
+        <f t="shared" si="2"/>
         <v>13.868750000045111</v>
       </c>
     </row>
@@ -7776,7 +7776,7 @@
         <v>43388.890277777798</v>
       </c>
       <c r="L141" s="6">
-        <f>K141-K$3</f>
+        <f t="shared" si="2"/>
         <v>18.240972222243727</v>
       </c>
     </row>
@@ -7812,7 +7812,7 @@
         <v>43388.890277777798</v>
       </c>
       <c r="L142" s="6">
-        <f>K142-K$3</f>
+        <f t="shared" si="2"/>
         <v>18.240972222243727</v>
       </c>
     </row>
@@ -7848,7 +7848,7 @@
         <v>43388.890277777798</v>
       </c>
       <c r="L143" s="6">
-        <f>K143-K$3</f>
+        <f t="shared" si="2"/>
         <v>18.240972222243727</v>
       </c>
     </row>
@@ -7884,7 +7884,7 @@
         <v>43388.890277777798</v>
       </c>
       <c r="L144" s="6">
-        <f>K144-K$3</f>
+        <f t="shared" si="2"/>
         <v>18.240972222243727</v>
       </c>
     </row>
@@ -7920,7 +7920,7 @@
         <v>43388.890277777798</v>
       </c>
       <c r="L145" s="6">
-        <f>K145-K$3</f>
+        <f t="shared" si="2"/>
         <v>18.240972222243727</v>
       </c>
     </row>
@@ -7956,7 +7956,7 @@
         <v>43388.890277777798</v>
       </c>
       <c r="L146" s="6">
-        <f>K146-K$3</f>
+        <f t="shared" si="2"/>
         <v>18.240972222243727</v>
       </c>
     </row>
@@ -7992,7 +7992,7 @@
         <v>43388.890277777798</v>
       </c>
       <c r="L147" s="6">
-        <f>K147-K$3</f>
+        <f t="shared" si="2"/>
         <v>18.240972222243727</v>
       </c>
     </row>
@@ -8028,7 +8028,7 @@
         <v>43388.890277777798</v>
       </c>
       <c r="L148" s="6">
-        <f>K148-K$3</f>
+        <f t="shared" si="2"/>
         <v>18.240972222243727</v>
       </c>
     </row>
@@ -8065,7 +8065,7 @@
         <v>43388.890277777798</v>
       </c>
       <c r="L149" s="6">
-        <f>K149-K$3</f>
+        <f t="shared" si="2"/>
         <v>18.240972222243727</v>
       </c>
     </row>
@@ -8102,7 +8102,7 @@
         <v>43388.890277777798</v>
       </c>
       <c r="L150" s="6">
-        <f>K150-K$3</f>
+        <f t="shared" si="2"/>
         <v>18.240972222243727</v>
       </c>
     </row>
@@ -8139,7 +8139,7 @@
         <v>43388.890277777798</v>
       </c>
       <c r="L151" s="6">
-        <f>K151-K$3</f>
+        <f t="shared" si="2"/>
         <v>18.240972222243727</v>
       </c>
     </row>
@@ -8175,7 +8175,7 @@
         <v>43388.890277777798</v>
       </c>
       <c r="L152" s="6">
-        <f>K152-K$3</f>
+        <f t="shared" si="2"/>
         <v>18.240972222243727</v>
       </c>
     </row>
@@ -8211,7 +8211,7 @@
         <v>43388.890277777798</v>
       </c>
       <c r="L153" s="6">
-        <f>K153-K$3</f>
+        <f t="shared" si="2"/>
         <v>18.240972222243727</v>
       </c>
     </row>
@@ -8247,7 +8247,7 @@
         <v>43388.890277777798</v>
       </c>
       <c r="L154" s="6">
-        <f>K154-K$3</f>
+        <f t="shared" si="2"/>
         <v>18.240972222243727</v>
       </c>
     </row>
@@ -8280,7 +8280,7 @@
         <v>43392.45</v>
       </c>
       <c r="L155" s="6">
-        <f>K155-K$3</f>
+        <f t="shared" si="2"/>
         <v>21.800694444442343</v>
       </c>
     </row>
@@ -8316,7 +8316,7 @@
         <v>43392.45</v>
       </c>
       <c r="L156" s="6">
-        <f>K156-K$3</f>
+        <f t="shared" si="2"/>
         <v>21.800694444442343</v>
       </c>
     </row>
@@ -8352,7 +8352,7 @@
         <v>43392.45</v>
       </c>
       <c r="L157" s="6">
-        <f>K157-K$3</f>
+        <f t="shared" si="2"/>
         <v>21.800694444442343</v>
       </c>
     </row>
@@ -8388,7 +8388,7 @@
         <v>43392.45</v>
       </c>
       <c r="L158" s="6">
-        <f>K158-K$3</f>
+        <f t="shared" si="2"/>
         <v>21.800694444442343</v>
       </c>
     </row>
@@ -8424,7 +8424,7 @@
         <v>43392.45</v>
       </c>
       <c r="L159" s="6">
-        <f>K159-K$3</f>
+        <f t="shared" si="2"/>
         <v>21.800694444442343</v>
       </c>
     </row>
@@ -8460,7 +8460,7 @@
         <v>43392.45</v>
       </c>
       <c r="L160" s="6">
-        <f>K160-K$3</f>
+        <f t="shared" si="2"/>
         <v>21.800694444442343</v>
       </c>
     </row>
@@ -8496,7 +8496,7 @@
         <v>43392.45</v>
       </c>
       <c r="L161" s="6">
-        <f>K161-K$3</f>
+        <f t="shared" si="2"/>
         <v>21.800694444442343</v>
       </c>
     </row>
@@ -8532,7 +8532,7 @@
         <v>43392.45</v>
       </c>
       <c r="L162" s="6">
-        <f>K162-K$3</f>
+        <f t="shared" si="2"/>
         <v>21.800694444442343</v>
       </c>
     </row>
@@ -8568,7 +8568,7 @@
         <v>43392.45</v>
       </c>
       <c r="L163" s="6">
-        <f>K163-K$3</f>
+        <f t="shared" si="2"/>
         <v>21.800694444442343</v>
       </c>
     </row>
@@ -8604,7 +8604,7 @@
         <v>43392.45</v>
       </c>
       <c r="L164" s="6">
-        <f>K164-K$3</f>
+        <f t="shared" si="2"/>
         <v>21.800694444442343</v>
       </c>
     </row>
@@ -8640,7 +8640,7 @@
         <v>43392.45</v>
       </c>
       <c r="L165" s="6">
-        <f>K165-K$3</f>
+        <f t="shared" si="2"/>
         <v>21.800694444442343</v>
       </c>
     </row>
@@ -8676,7 +8676,7 @@
         <v>43392.45</v>
       </c>
       <c r="L166" s="6">
-        <f>K166-K$3</f>
+        <f t="shared" si="2"/>
         <v>21.800694444442343</v>
       </c>
     </row>
@@ -8712,7 +8712,7 @@
         <v>43392.45</v>
       </c>
       <c r="L167" s="6">
-        <f>K167-K$3</f>
+        <f t="shared" si="2"/>
         <v>21.800694444442343</v>
       </c>
     </row>
@@ -8748,7 +8748,7 @@
         <v>43392.45</v>
       </c>
       <c r="L168" s="6">
-        <f>K168-K$3</f>
+        <f t="shared" si="2"/>
         <v>21.800694444442343</v>
       </c>
     </row>
@@ -8781,7 +8781,7 @@
         <v>43398.588888888902</v>
       </c>
       <c r="L169" s="6">
-        <f>K169-K$3</f>
+        <f t="shared" si="2"/>
         <v>27.9395833333474</v>
       </c>
     </row>
@@ -8817,7 +8817,7 @@
         <v>43398.588888888902</v>
       </c>
       <c r="L170" s="6">
-        <f>K170-K$3</f>
+        <f t="shared" si="2"/>
         <v>27.9395833333474</v>
       </c>
     </row>
@@ -8853,7 +8853,7 @@
         <v>43398.588888888902</v>
       </c>
       <c r="L171" s="6">
-        <f>K171-K$3</f>
+        <f t="shared" si="2"/>
         <v>27.9395833333474</v>
       </c>
     </row>
@@ -8889,7 +8889,7 @@
         <v>43398.588888888902</v>
       </c>
       <c r="L172" s="6">
-        <f>K172-K$3</f>
+        <f t="shared" si="2"/>
         <v>27.9395833333474</v>
       </c>
     </row>
@@ -8925,7 +8925,7 @@
         <v>43398.588888888902</v>
       </c>
       <c r="L173" s="6">
-        <f>K173-K$3</f>
+        <f t="shared" si="2"/>
         <v>27.9395833333474</v>
       </c>
     </row>
@@ -8961,7 +8961,7 @@
         <v>43398.588888888902</v>
       </c>
       <c r="L174" s="6">
-        <f>K174-K$3</f>
+        <f t="shared" si="2"/>
         <v>27.9395833333474</v>
       </c>
     </row>
@@ -8997,7 +8997,7 @@
         <v>43398.588888888902</v>
       </c>
       <c r="L175" s="6">
-        <f>K175-K$3</f>
+        <f t="shared" si="2"/>
         <v>27.9395833333474</v>
       </c>
     </row>
@@ -9033,7 +9033,7 @@
         <v>43398.588888888902</v>
       </c>
       <c r="L176" s="6">
-        <f>K176-K$3</f>
+        <f t="shared" si="2"/>
         <v>27.9395833333474</v>
       </c>
     </row>
@@ -9069,7 +9069,7 @@
         <v>43398.588888888902</v>
       </c>
       <c r="L177" s="6">
-        <f>K177-K$3</f>
+        <f t="shared" si="2"/>
         <v>27.9395833333474</v>
       </c>
     </row>
@@ -9105,7 +9105,7 @@
         <v>43398.588888888902</v>
       </c>
       <c r="L178" s="6">
-        <f>K178-K$3</f>
+        <f t="shared" si="2"/>
         <v>27.9395833333474</v>
       </c>
     </row>
@@ -9141,7 +9141,7 @@
         <v>43398.588888888902</v>
       </c>
       <c r="L179" s="6">
-        <f>K179-K$3</f>
+        <f t="shared" si="2"/>
         <v>27.9395833333474</v>
       </c>
     </row>
@@ -9177,7 +9177,7 @@
         <v>43398.588888888902</v>
       </c>
       <c r="L180" s="6">
-        <f>K180-K$3</f>
+        <f t="shared" si="2"/>
         <v>27.9395833333474</v>
       </c>
     </row>
@@ -9213,7 +9213,7 @@
         <v>43398.588888888902</v>
       </c>
       <c r="L181" s="6">
-        <f>K181-K$3</f>
+        <f t="shared" si="2"/>
         <v>27.9395833333474</v>
       </c>
     </row>
@@ -9249,7 +9249,7 @@
         <v>43398.588888888902</v>
       </c>
       <c r="L182" s="6">
-        <f>K182-K$3</f>
+        <f t="shared" si="2"/>
         <v>27.9395833333474</v>
       </c>
     </row>
@@ -9283,7 +9283,7 @@
         <v>43402.406944444498</v>
       </c>
       <c r="L183" s="6">
-        <f>K183-K$3</f>
+        <f t="shared" si="2"/>
         <v>31.757638888942893</v>
       </c>
     </row>
@@ -9319,7 +9319,7 @@
         <v>43402.406944444498</v>
       </c>
       <c r="L184" s="6">
-        <f>K184-K$3</f>
+        <f t="shared" si="2"/>
         <v>31.757638888942893</v>
       </c>
     </row>
@@ -9355,7 +9355,7 @@
         <v>43402.406944444498</v>
       </c>
       <c r="L185" s="6">
-        <f>K185-K$3</f>
+        <f t="shared" si="2"/>
         <v>31.757638888942893</v>
       </c>
     </row>
@@ -9391,7 +9391,7 @@
         <v>43402.406944444498</v>
       </c>
       <c r="L186" s="6">
-        <f>K186-K$3</f>
+        <f t="shared" si="2"/>
         <v>31.757638888942893</v>
       </c>
     </row>
@@ -9427,7 +9427,7 @@
         <v>43402.406944444498</v>
       </c>
       <c r="L187" s="6">
-        <f>K187-K$3</f>
+        <f t="shared" si="2"/>
         <v>31.757638888942893</v>
       </c>
     </row>
@@ -9463,7 +9463,7 @@
         <v>43402.406944444498</v>
       </c>
       <c r="L188" s="6">
-        <f>K188-K$3</f>
+        <f t="shared" si="2"/>
         <v>31.757638888942893</v>
       </c>
     </row>
@@ -9499,7 +9499,7 @@
         <v>43402.406944444498</v>
       </c>
       <c r="L189" s="6">
-        <f>K189-K$3</f>
+        <f t="shared" si="2"/>
         <v>31.757638888942893</v>
       </c>
     </row>
@@ -9535,7 +9535,7 @@
         <v>43402.406944444498</v>
       </c>
       <c r="L190" s="6">
-        <f>K190-K$3</f>
+        <f t="shared" si="2"/>
         <v>31.757638888942893</v>
       </c>
     </row>
@@ -9571,7 +9571,7 @@
         <v>43402.406944444498</v>
       </c>
       <c r="L191" s="6">
-        <f>K191-K$3</f>
+        <f t="shared" si="2"/>
         <v>31.757638888942893</v>
       </c>
     </row>
@@ -9607,7 +9607,7 @@
         <v>43402.406944444498</v>
       </c>
       <c r="L192" s="6">
-        <f>K192-K$3</f>
+        <f t="shared" si="2"/>
         <v>31.757638888942893</v>
       </c>
     </row>
@@ -9643,7 +9643,7 @@
         <v>43402.406944444498</v>
       </c>
       <c r="L193" s="6">
-        <f>K193-K$3</f>
+        <f t="shared" si="2"/>
         <v>31.757638888942893</v>
       </c>
     </row>
@@ -9679,7 +9679,7 @@
         <v>43402.406944444498</v>
       </c>
       <c r="L194" s="6">
-        <f>K194-K$3</f>
+        <f t="shared" si="2"/>
         <v>31.757638888942893</v>
       </c>
     </row>
@@ -9715,7 +9715,7 @@
         <v>43402.406944444498</v>
       </c>
       <c r="L195" s="6">
-        <f>K195-K$3</f>
+        <f t="shared" ref="L195:L258" si="3">K195-K$3</f>
         <v>31.757638888942893</v>
       </c>
     </row>
@@ -9751,7 +9751,7 @@
         <v>43402.406944444498</v>
       </c>
       <c r="L196" s="6">
-        <f>K196-K$3</f>
+        <f t="shared" si="3"/>
         <v>31.757638888942893</v>
       </c>
     </row>
@@ -9787,7 +9787,7 @@
         <v>43420.588194444397</v>
       </c>
       <c r="L197" s="6">
-        <f>K197-K$3</f>
+        <f t="shared" si="3"/>
         <v>49.938888888842484</v>
       </c>
     </row>
@@ -9826,7 +9826,7 @@
         <v>43420.588194444397</v>
       </c>
       <c r="L198" s="6">
-        <f>K198-K$3</f>
+        <f t="shared" si="3"/>
         <v>49.938888888842484</v>
       </c>
     </row>
@@ -9865,7 +9865,7 @@
         <v>43420.588194444397</v>
       </c>
       <c r="L199" s="6">
-        <f>K199-K$3</f>
+        <f t="shared" si="3"/>
         <v>49.938888888842484</v>
       </c>
     </row>
@@ -9904,7 +9904,7 @@
         <v>43420.588194444397</v>
       </c>
       <c r="L200" s="6">
-        <f>K200-K$3</f>
+        <f t="shared" si="3"/>
         <v>49.938888888842484</v>
       </c>
     </row>
@@ -9944,7 +9944,7 @@
         <v>43420.588194444397</v>
       </c>
       <c r="L201" s="6">
-        <f>K201-K$3</f>
+        <f t="shared" si="3"/>
         <v>49.938888888842484</v>
       </c>
     </row>
@@ -9984,7 +9984,7 @@
         <v>43420.588194444397</v>
       </c>
       <c r="L202" s="6">
-        <f>K202-K$3</f>
+        <f t="shared" si="3"/>
         <v>49.938888888842484</v>
       </c>
     </row>
@@ -10023,7 +10023,7 @@
         <v>43420.588194444397</v>
       </c>
       <c r="L203" s="6">
-        <f>K203-K$3</f>
+        <f t="shared" si="3"/>
         <v>49.938888888842484</v>
       </c>
     </row>
@@ -10062,7 +10062,7 @@
         <v>43420.588194444397</v>
       </c>
       <c r="L204" s="6">
-        <f>K204-K$3</f>
+        <f t="shared" si="3"/>
         <v>49.938888888842484</v>
       </c>
     </row>
@@ -10101,7 +10101,7 @@
         <v>43420.588194444397</v>
       </c>
       <c r="L205" s="6">
-        <f>K205-K$3</f>
+        <f t="shared" si="3"/>
         <v>49.938888888842484</v>
       </c>
     </row>
@@ -10140,7 +10140,7 @@
         <v>43420.588194444397</v>
       </c>
       <c r="L206" s="6">
-        <f>K206-K$3</f>
+        <f t="shared" si="3"/>
         <v>49.938888888842484</v>
       </c>
     </row>
@@ -10179,7 +10179,7 @@
         <v>43420.588194444397</v>
       </c>
       <c r="L207" s="6">
-        <f>K207-K$3</f>
+        <f t="shared" si="3"/>
         <v>49.938888888842484</v>
       </c>
     </row>
@@ -10218,7 +10218,7 @@
         <v>43420.588194444397</v>
       </c>
       <c r="L208" s="6">
-        <f>K208-K$3</f>
+        <f t="shared" si="3"/>
         <v>49.938888888842484</v>
       </c>
     </row>
@@ -10257,7 +10257,7 @@
         <v>43420.588194444397</v>
       </c>
       <c r="L209" s="6">
-        <f>K209-K$3</f>
+        <f t="shared" si="3"/>
         <v>49.938888888842484</v>
       </c>
     </row>
@@ -10296,7 +10296,7 @@
         <v>43420.588194444397</v>
       </c>
       <c r="L210" s="6">
-        <f>K210-K$3</f>
+        <f t="shared" si="3"/>
         <v>49.938888888842484</v>
       </c>
     </row>
@@ -10332,7 +10332,7 @@
         <v>43451.484722222202</v>
       </c>
       <c r="L211" s="6">
-        <f>K211-K$3</f>
+        <f t="shared" si="3"/>
         <v>80.835416666646779</v>
       </c>
     </row>
@@ -10368,7 +10368,7 @@
         <v>43451.484722222202</v>
       </c>
       <c r="L212" s="6">
-        <f>K212-K$3</f>
+        <f t="shared" si="3"/>
         <v>80.835416666646779</v>
       </c>
     </row>
@@ -10404,7 +10404,7 @@
         <v>43451.484722222202</v>
       </c>
       <c r="L213" s="6">
-        <f>K213-K$3</f>
+        <f t="shared" si="3"/>
         <v>80.835416666646779</v>
       </c>
     </row>
@@ -10440,7 +10440,7 @@
         <v>43451.484722222202</v>
       </c>
       <c r="L214" s="6">
-        <f>K214-K$3</f>
+        <f t="shared" si="3"/>
         <v>80.835416666646779</v>
       </c>
     </row>
@@ -10476,7 +10476,7 @@
         <v>43451.484722222202</v>
       </c>
       <c r="L215" s="6">
-        <f>K215-K$3</f>
+        <f t="shared" si="3"/>
         <v>80.835416666646779</v>
       </c>
     </row>
@@ -10512,7 +10512,7 @@
         <v>43451.484722222202</v>
       </c>
       <c r="L216" s="6">
-        <f>K216-K$3</f>
+        <f t="shared" si="3"/>
         <v>80.835416666646779</v>
       </c>
     </row>
@@ -10548,7 +10548,7 @@
         <v>43451.484722222202</v>
       </c>
       <c r="L217" s="6">
-        <f>K217-K$3</f>
+        <f t="shared" si="3"/>
         <v>80.835416666646779</v>
       </c>
     </row>
@@ -10585,7 +10585,7 @@
         <v>43451.484722222202</v>
       </c>
       <c r="L218" s="6">
-        <f>K218-K$3</f>
+        <f t="shared" si="3"/>
         <v>80.835416666646779</v>
       </c>
     </row>
@@ -10622,7 +10622,7 @@
         <v>43451.484722222202</v>
       </c>
       <c r="L219" s="6">
-        <f>K219-K$3</f>
+        <f t="shared" si="3"/>
         <v>80.835416666646779</v>
       </c>
     </row>
@@ -10659,7 +10659,7 @@
         <v>43451.484722222202</v>
       </c>
       <c r="L220" s="6">
-        <f>K220-K$3</f>
+        <f t="shared" si="3"/>
         <v>80.835416666646779</v>
       </c>
     </row>
@@ -10696,7 +10696,7 @@
         <v>43451.484722222202</v>
       </c>
       <c r="L221" s="6">
-        <f>K221-K$3</f>
+        <f t="shared" si="3"/>
         <v>80.835416666646779</v>
       </c>
     </row>
@@ -10732,7 +10732,7 @@
         <v>43451.484722222202</v>
       </c>
       <c r="L222" s="6">
-        <f>K222-K$3</f>
+        <f t="shared" si="3"/>
         <v>80.835416666646779</v>
       </c>
     </row>
@@ -10768,7 +10768,7 @@
         <v>43451.484722222202</v>
       </c>
       <c r="L223" s="6">
-        <f>K223-K$3</f>
+        <f t="shared" si="3"/>
         <v>80.835416666646779</v>
       </c>
     </row>
@@ -10804,7 +10804,7 @@
         <v>43451.484722222202</v>
       </c>
       <c r="L224" s="6">
-        <f>K224-K$3</f>
+        <f t="shared" si="3"/>
         <v>80.835416666646779</v>
       </c>
     </row>
@@ -10837,7 +10837,7 @@
         <v>43499.548611111109</v>
       </c>
       <c r="L225" s="6">
-        <f>K225-K$3</f>
+        <f t="shared" si="3"/>
         <v>128.89930555555475</v>
       </c>
     </row>
@@ -10873,7 +10873,7 @@
         <v>43499.548611111109</v>
       </c>
       <c r="L226" s="6">
-        <f>K226-K$3</f>
+        <f t="shared" si="3"/>
         <v>128.89930555555475</v>
       </c>
     </row>
@@ -10909,7 +10909,7 @@
         <v>43499.548611111109</v>
       </c>
       <c r="L227" s="6">
-        <f>K227-K$3</f>
+        <f t="shared" si="3"/>
         <v>128.89930555555475</v>
       </c>
     </row>
@@ -10948,7 +10948,7 @@
         <v>43499.548611111109</v>
       </c>
       <c r="L228" s="6">
-        <f>K228-K$3</f>
+        <f t="shared" si="3"/>
         <v>128.89930555555475</v>
       </c>
     </row>
@@ -10985,7 +10985,7 @@
         <v>43499.548611111109</v>
       </c>
       <c r="L229" s="6">
-        <f>K229-K$3</f>
+        <f t="shared" si="3"/>
         <v>128.89930555555475</v>
       </c>
     </row>
@@ -11022,7 +11022,7 @@
         <v>43499.548611111109</v>
       </c>
       <c r="L230" s="6">
-        <f>K230-K$3</f>
+        <f t="shared" si="3"/>
         <v>128.89930555555475</v>
       </c>
     </row>
@@ -11059,7 +11059,7 @@
         <v>43499.548611111109</v>
       </c>
       <c r="L231" s="6">
-        <f>K231-K$3</f>
+        <f t="shared" si="3"/>
         <v>128.89930555555475</v>
       </c>
     </row>
@@ -11096,7 +11096,7 @@
         <v>43499.548611111109</v>
       </c>
       <c r="L232" s="6">
-        <f>K232-K$3</f>
+        <f t="shared" si="3"/>
         <v>128.89930555555475</v>
       </c>
     </row>
@@ -11132,7 +11132,7 @@
         <v>43499.548611111109</v>
       </c>
       <c r="L233" s="6">
-        <f>K233-K$3</f>
+        <f t="shared" si="3"/>
         <v>128.89930555555475</v>
       </c>
     </row>
@@ -11168,7 +11168,7 @@
         <v>43499.548611111109</v>
       </c>
       <c r="L234" s="6">
-        <f>K234-K$3</f>
+        <f t="shared" si="3"/>
         <v>128.89930555555475</v>
       </c>
     </row>
@@ -11204,7 +11204,7 @@
         <v>43499.548611111109</v>
       </c>
       <c r="L235" s="6">
-        <f>K235-K$3</f>
+        <f t="shared" si="3"/>
         <v>128.89930555555475</v>
       </c>
     </row>
@@ -11240,7 +11240,7 @@
         <v>43499.548611111109</v>
       </c>
       <c r="L236" s="6">
-        <f>K236-K$3</f>
+        <f t="shared" si="3"/>
         <v>128.89930555555475</v>
       </c>
     </row>
@@ -11276,7 +11276,7 @@
         <v>43499.548611111109</v>
       </c>
       <c r="L237" s="6">
-        <f>K237-K$3</f>
+        <f t="shared" si="3"/>
         <v>128.89930555555475</v>
       </c>
     </row>
@@ -11312,7 +11312,7 @@
         <v>43499.548611111109</v>
       </c>
       <c r="L238" s="6">
-        <f>K238-K$3</f>
+        <f t="shared" si="3"/>
         <v>128.89930555555475</v>
       </c>
     </row>
@@ -11334,7 +11334,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fix typo in L1 Dec 2018 vol data
</commit_message>
<xml_diff>
--- a/experiments/IISBMP2/data/biogas_and_setup.xlsx
+++ b/experiments/IISBMP2/data/biogas_and_setup.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="11_BA913473D9CE20ABDCCA9BC8D11D853CACE05D5F" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16395" windowHeight="8190" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16395" windowHeight="8190" tabRatio="500" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="1" r:id="rId1"/>
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1143" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1151" uniqueCount="173">
   <si>
     <t>Experiment</t>
   </si>
@@ -591,6 +591,15 @@
   </si>
   <si>
     <t>Change inoculum only to inoculum in setup$descrip</t>
+  </si>
+  <si>
+    <t>12 March 2019</t>
+  </si>
+  <si>
+    <t>Biogas sheet L1 2 Oct 2018, filled in mass.init with previous mass.final value</t>
+  </si>
+  <si>
+    <t>Biogas sheet L1 17 Dec 2018, corrected typo in mass.init (was .68)</t>
   </si>
 </sst>
 </file>
@@ -2494,9 +2503,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMK240"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0" xr3:uid="{958C4451-9541-5A59-BF78-D2F731DF1C81}">
-      <pane xSplit="1" ySplit="2" topLeftCell="B49" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="J74" sqref="J74"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0" xr3:uid="{958C4451-9541-5A59-BF78-D2F731DF1C81}">
+      <pane xSplit="1" ySplit="2" topLeftCell="B195" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="G222" sqref="G222"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
     </sheetView>
@@ -10724,7 +10733,7 @@
         <v>1010.47</v>
       </c>
       <c r="G222" s="1">
-        <v>465.68</v>
+        <v>465.48</v>
       </c>
       <c r="H222" s="10">
         <v>92</v>
@@ -11336,10 +11345,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AMK17"/>
+  <dimension ref="A1:AMK19"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0" xr3:uid="{842E5F09-E766-5B8D-85AF-A39847EA96FD}">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0" xr3:uid="{842E5F09-E766-5B8D-85AF-A39847EA96FD}">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -11589,6 +11598,34 @@
         <v>169</v>
       </c>
     </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="17" t="s">
+        <v>170</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="17" t="s">
+        <v>170</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>172</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Correct data entry typo for C3
</commit_message>
<xml_diff>
--- a/experiments/IISBMP2/data/biogas_and_setup.xlsx
+++ b/experiments/IISBMP2/data/biogas_and_setup.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="11_BA913473D9CE20ABDCCA9BC8D11D853CACE05D5F" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16395" windowHeight="8190" tabRatio="500" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16395" windowHeight="8190" tabRatio="500" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="1" r:id="rId1"/>
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1151" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1155" uniqueCount="174">
   <si>
     <t>Experiment</t>
   </si>
@@ -600,6 +600,9 @@
   </si>
   <si>
     <t>Biogas sheet L1 17 Dec 2018, corrected typo in mass.init (was .68)</t>
+  </si>
+  <si>
+    <t>Biogas sheet C3 28 Sept 2018, correct typo in mass.final (was .25)</t>
   </si>
 </sst>
 </file>
@@ -2504,8 +2507,8 @@
   <dimension ref="A1:AMK240"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0" xr3:uid="{958C4451-9541-5A59-BF78-D2F731DF1C81}">
-      <pane xSplit="1" ySplit="2" topLeftCell="B195" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="G222" sqref="G222"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="I19" sqref="I19"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
     </sheetView>
@@ -3266,7 +3269,7 @@
         <v>202</v>
       </c>
       <c r="I19" s="8">
-        <v>468.25</v>
+        <v>468.05</v>
       </c>
       <c r="K19" s="11">
         <v>43371.375</v>
@@ -11345,10 +11348,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AMK19"/>
+  <dimension ref="A1:AMK20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0" xr3:uid="{842E5F09-E766-5B8D-85AF-A39847EA96FD}">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -11626,6 +11629,20 @@
         <v>172</v>
       </c>
     </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="17" t="s">
+        <v>170</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>173</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Corrections to data file (again), restore corrected version from yesterday w L1 L2 & C3 corrections, Dropbox error?
</commit_message>
<xml_diff>
--- a/experiments/IISBMP2/data/biogas_and_setup.xlsx
+++ b/experiments/IISBMP2/data/biogas_and_setup.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="11_BA913473D9CE20ABDCCA9BC8D11D853CACE05D5F" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16395" windowHeight="8190" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16395" windowHeight="8190" tabRatio="500" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="1" r:id="rId1"/>
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1143" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1155" uniqueCount="174">
   <si>
     <t>Experiment</t>
   </si>
@@ -591,6 +591,18 @@
   </si>
   <si>
     <t>Change inoculum only to inoculum in setup$descrip</t>
+  </si>
+  <si>
+    <t>12 March 2019</t>
+  </si>
+  <si>
+    <t>Biogas sheet L1 2 Oct 2018, filled in mass.init with previous mass.final value</t>
+  </si>
+  <si>
+    <t>Biogas sheet L1 17 Dec 2018, corrected typo in mass.init (was .68)</t>
+  </si>
+  <si>
+    <t>Biogas sheet C3 28 Sept 2018, correct typo in mass.final (was .25)</t>
   </si>
 </sst>
 </file>
@@ -2494,9 +2506,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMK240"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0" xr3:uid="{958C4451-9541-5A59-BF78-D2F731DF1C81}">
-      <pane xSplit="1" ySplit="2" topLeftCell="B49" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="J74" sqref="J74"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0" xr3:uid="{958C4451-9541-5A59-BF78-D2F731DF1C81}">
+      <pane xSplit="1" ySplit="2" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="I19" sqref="I19"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
     </sheetView>
@@ -3257,7 +3269,7 @@
         <v>202</v>
       </c>
       <c r="I19" s="8">
-        <v>468.25</v>
+        <v>468.05</v>
       </c>
       <c r="K19" s="11">
         <v>43371.375</v>
@@ -10724,7 +10736,7 @@
         <v>1010.47</v>
       </c>
       <c r="G222" s="1">
-        <v>465.68</v>
+        <v>465.48</v>
       </c>
       <c r="H222" s="10">
         <v>92</v>
@@ -11336,10 +11348,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AMK17"/>
+  <dimension ref="A1:AMK20"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0" xr3:uid="{842E5F09-E766-5B8D-85AF-A39847EA96FD}">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0" xr3:uid="{842E5F09-E766-5B8D-85AF-A39847EA96FD}">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -11589,6 +11601,48 @@
         <v>169</v>
       </c>
     </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="17" t="s">
+        <v>170</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="17" t="s">
+        <v>170</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="17" t="s">
+        <v>170</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>173</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Add measurements for 07.04.19
</commit_message>
<xml_diff>
--- a/experiments/IISBMP2/data/biogas_and_setup.xlsx
+++ b/experiments/IISBMP2/data/biogas_and_setup.xlsx
@@ -9,14 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16395" windowHeight="8190" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16395" windowHeight="8190" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="1" r:id="rId1"/>
     <sheet name="Biogas" sheetId="2" r:id="rId2"/>
     <sheet name="ChangeLog" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913" iterate="1" iterateDelta="1E-4"/>
+  <calcPr calcId="162913" iterate="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1174" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1221" uniqueCount="183">
   <si>
     <t>Experiment</t>
   </si>
@@ -617,6 +617,18 @@
   </si>
   <si>
     <t>28 March 2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add sampling data for 07 april 2019. </t>
+  </si>
+  <si>
+    <t>07 April 2019</t>
+  </si>
+  <si>
+    <t>07.04.2019</t>
+  </si>
+  <si>
+    <t>Forgot to write down initial mass. Set to final value from previous (assumes no leakage).</t>
   </si>
 </sst>
 </file>
@@ -628,7 +640,7 @@
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="mm/dd/yy"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -661,6 +673,13 @@
       <name val="Tahoma"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -682,7 +701,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -732,6 +751,9 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2563,13 +2585,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK240"/>
+  <dimension ref="A1:AMK252"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B222" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I19" sqref="I19"/>
+      <selection pane="bottomRight" activeCell="L246" sqref="L246"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -11392,10 +11414,414 @@
       </c>
     </row>
     <row r="239" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A239" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B239" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C239" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="D239" s="8">
+        <v>11.09</v>
+      </c>
+      <c r="E239" s="10">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="F239" s="8">
+        <v>1004.06</v>
+      </c>
+      <c r="G239" s="1">
+        <v>487.56</v>
+      </c>
       <c r="L239" s="6"/>
     </row>
     <row r="240" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A240" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B240" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C240" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="D240" s="8">
+        <v>11.09</v>
+      </c>
+      <c r="E240" s="10">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="F240" s="8">
+        <v>1004.06</v>
+      </c>
+      <c r="G240" s="1">
+        <v>467.35</v>
+      </c>
+      <c r="H240" s="10">
+        <v>97</v>
+      </c>
+      <c r="I240" s="8">
+        <v>467.24</v>
+      </c>
       <c r="L240" s="6"/>
+    </row>
+    <row r="241" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A241" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B241" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C241" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="D241" s="8">
+        <v>11.09</v>
+      </c>
+      <c r="E241" s="10">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="F241" s="8">
+        <v>1004.06</v>
+      </c>
+      <c r="G241" s="1">
+        <v>468.33</v>
+      </c>
+      <c r="H241" s="10">
+        <v>97</v>
+      </c>
+      <c r="I241" s="8">
+        <v>468.22</v>
+      </c>
+    </row>
+    <row r="242" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A242" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B242" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C242" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="D242" s="8">
+        <v>11.09</v>
+      </c>
+      <c r="E242" s="10">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="F242" s="8">
+        <v>1004.06</v>
+      </c>
+      <c r="G242" s="1">
+        <v>468.73</v>
+      </c>
+      <c r="H242" s="10">
+        <v>101</v>
+      </c>
+      <c r="I242" s="8">
+        <v>468.61</v>
+      </c>
+    </row>
+    <row r="243" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A243" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B243" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C243" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="D243" s="8">
+        <v>11.09</v>
+      </c>
+      <c r="E243" s="10">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="F243" s="8">
+        <v>1004.06</v>
+      </c>
+      <c r="G243" s="1">
+        <v>465.82</v>
+      </c>
+      <c r="H243" s="10">
+        <v>82</v>
+      </c>
+      <c r="I243" s="8">
+        <v>465.74</v>
+      </c>
+    </row>
+    <row r="244" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A244" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B244" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C244" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="D244" s="8">
+        <v>11.09</v>
+      </c>
+      <c r="E244" s="10">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="F244" s="8">
+        <v>1004.06</v>
+      </c>
+      <c r="G244" s="1">
+        <v>469.17</v>
+      </c>
+      <c r="H244" s="10">
+        <v>77</v>
+      </c>
+      <c r="I244" s="8">
+        <v>469.09</v>
+      </c>
+    </row>
+    <row r="245" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A245" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B245" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C245" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="D245" s="8">
+        <v>11.09</v>
+      </c>
+      <c r="E245" s="10">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="F245" s="8">
+        <v>1004.06</v>
+      </c>
+      <c r="G245" s="1">
+        <v>465.6</v>
+      </c>
+      <c r="H245" s="10">
+        <v>75</v>
+      </c>
+      <c r="I245" s="8">
+        <v>465.51</v>
+      </c>
+    </row>
+    <row r="246" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A246" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B246" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C246" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="D246" s="8">
+        <v>11.09</v>
+      </c>
+      <c r="E246" s="10">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="F246" s="8">
+        <v>1004.06</v>
+      </c>
+      <c r="G246" s="1">
+        <v>465.16</v>
+      </c>
+      <c r="H246" s="10">
+        <v>77</v>
+      </c>
+      <c r="I246" s="8">
+        <v>465.08</v>
+      </c>
+    </row>
+    <row r="247" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A247" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B247" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C247" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="D247" s="8">
+        <v>11.09</v>
+      </c>
+      <c r="E247" s="10">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="F247" s="8">
+        <v>1004.06</v>
+      </c>
+      <c r="G247" s="1">
+        <v>465.89</v>
+      </c>
+      <c r="H247" s="10">
+        <v>81</v>
+      </c>
+      <c r="I247" s="8">
+        <v>465.82</v>
+      </c>
+    </row>
+    <row r="248" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A248" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B248" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C248" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="D248" s="8">
+        <v>11.09</v>
+      </c>
+      <c r="E248" s="10">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="F248" s="8">
+        <v>1004.06</v>
+      </c>
+      <c r="G248" s="1">
+        <v>467.91</v>
+      </c>
+      <c r="H248" s="10">
+        <v>78</v>
+      </c>
+      <c r="I248" s="8">
+        <v>467.82</v>
+      </c>
+    </row>
+    <row r="249" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A249" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B249" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C249" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="D249" s="8">
+        <v>11.09</v>
+      </c>
+      <c r="E249" s="10">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="F249" s="8">
+        <v>1004.06</v>
+      </c>
+      <c r="G249" s="1">
+        <v>727.5</v>
+      </c>
+      <c r="H249" s="10">
+        <f>144+42</f>
+        <v>186</v>
+      </c>
+      <c r="I249" s="8">
+        <v>727.33</v>
+      </c>
+    </row>
+    <row r="250" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A250" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B250" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C250" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="D250" s="8">
+        <v>11.09</v>
+      </c>
+      <c r="E250" s="10">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="F250" s="8">
+        <v>1004.06</v>
+      </c>
+      <c r="G250" s="1">
+        <v>720.07</v>
+      </c>
+      <c r="H250" s="10">
+        <f>145+43</f>
+        <v>188</v>
+      </c>
+      <c r="I250" s="8">
+        <v>719.88</v>
+      </c>
+    </row>
+    <row r="251" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A251" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B251" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C251" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="D251" s="8">
+        <v>11.09</v>
+      </c>
+      <c r="E251" s="10">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="F251" s="8">
+        <v>1004.06</v>
+      </c>
+      <c r="G251" s="1">
+        <v>738.41</v>
+      </c>
+      <c r="H251" s="10">
+        <f>143+46</f>
+        <v>189</v>
+      </c>
+      <c r="I251" s="8">
+        <v>738.23</v>
+      </c>
+    </row>
+    <row r="252" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A252" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B252" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C252" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="D252" s="8">
+        <v>11.09</v>
+      </c>
+      <c r="E252" s="10">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="F252" s="8">
+        <v>1004.06</v>
+      </c>
+      <c r="G252" s="19">
+        <f>I232</f>
+        <v>721.94</v>
+      </c>
+      <c r="H252" s="10">
+        <f>171+13</f>
+        <v>184</v>
+      </c>
+      <c r="I252" s="8">
+        <v>721.59</v>
+      </c>
+      <c r="J252" s="2" t="s">
+        <v>182</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -11407,10 +11833,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK21"/>
+  <dimension ref="A1:AMK22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -11716,6 +12142,20 @@
         <v>177</v>
       </c>
     </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="17" t="s">
+        <v>180</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>179</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Add GD comparison plot for appendix for exper D. Change LBD to LB in data
</commit_message>
<xml_diff>
--- a/experiments/IISBMP2/data/biogas_and_setup.xlsx
+++ b/experiments/IISBMP2/data/biogas_and_setup.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16395" windowHeight="8190" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16395" windowHeight="8190" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="1" r:id="rId1"/>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1221" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1225" uniqueCount="185">
   <si>
     <t>Experiment</t>
   </si>
@@ -610,9 +610,6 @@
     <t>descrip1</t>
   </si>
   <si>
-    <t>LBD</t>
-  </si>
-  <si>
     <t>Add new description column</t>
   </si>
   <si>
@@ -629,6 +626,15 @@
   </si>
   <si>
     <t>Forgot to write down initial mass. Set to final value from previous (assumes no leakage).</t>
+  </si>
+  <si>
+    <t>LB</t>
+  </si>
+  <si>
+    <t>1 April 2019</t>
+  </si>
+  <si>
+    <t>Change name of LBD to LB in descrip</t>
   </si>
 </sst>
 </file>
@@ -1502,7 +1508,7 @@
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D17" sqref="D17"/>
+      <selection pane="bottomRight" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1867,7 +1873,7 @@
         <v>46</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>47</v>
@@ -1939,7 +1945,7 @@
         <v>50</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>47</v>
@@ -2011,7 +2017,7 @@
         <v>51</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>47</v>
@@ -2587,8 +2593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK252"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B222" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B207" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="L246" sqref="L246"/>
@@ -11421,7 +11427,7 @@
         <v>63</v>
       </c>
       <c r="C239" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D239" s="8">
         <v>11.09</v>
@@ -11445,7 +11451,7 @@
         <v>46</v>
       </c>
       <c r="C240" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D240" s="8">
         <v>11.09</v>
@@ -11475,7 +11481,7 @@
         <v>50</v>
       </c>
       <c r="C241" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D241" s="8">
         <v>11.09</v>
@@ -11504,7 +11510,7 @@
         <v>51</v>
       </c>
       <c r="C242" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D242" s="8">
         <v>11.09</v>
@@ -11533,7 +11539,7 @@
         <v>41</v>
       </c>
       <c r="C243" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D243" s="8">
         <v>11.09</v>
@@ -11562,7 +11568,7 @@
         <v>44</v>
       </c>
       <c r="C244" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D244" s="8">
         <v>11.09</v>
@@ -11591,7 +11597,7 @@
         <v>45</v>
       </c>
       <c r="C245" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D245" s="8">
         <v>11.09</v>
@@ -11620,7 +11626,7 @@
         <v>52</v>
       </c>
       <c r="C246" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D246" s="8">
         <v>11.09</v>
@@ -11649,7 +11655,7 @@
         <v>55</v>
       </c>
       <c r="C247" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D247" s="8">
         <v>11.09</v>
@@ -11678,7 +11684,7 @@
         <v>56</v>
       </c>
       <c r="C248" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D248" s="8">
         <v>11.09</v>
@@ -11707,7 +11713,7 @@
         <v>57</v>
       </c>
       <c r="C249" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D249" s="8">
         <v>11.09</v>
@@ -11737,7 +11743,7 @@
         <v>60</v>
       </c>
       <c r="C250" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D250" s="8">
         <v>11.09</v>
@@ -11767,7 +11773,7 @@
         <v>61</v>
       </c>
       <c r="C251" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D251" s="8">
         <v>11.09</v>
@@ -11797,7 +11803,7 @@
         <v>62</v>
       </c>
       <c r="C252" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D252" s="8">
         <v>11.09</v>
@@ -11820,7 +11826,7 @@
         <v>721.59</v>
       </c>
       <c r="J252" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -11833,10 +11839,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK22"/>
+  <dimension ref="A1:AMK23"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12130,7 +12136,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="17" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>142</v>
@@ -12139,12 +12145,12 @@
         <v>148</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="17" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>142</v>
@@ -12153,7 +12159,21 @@
         <v>148</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="17" t="s">
+        <v>183</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>184</v>
       </c>
     </row>
   </sheetData>

</xml_diff>